<commit_message>
Finalised Heuristic program for left-overs
</commit_message>
<xml_diff>
--- a/Azores_Flight_Data_v2.xlsx
+++ b/Azores_Flight_Data_v2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nils de Krom\Desktop\Operations Optimisation Assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nils de Krom\Documents\GitHub\Operations_optimization_assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF02615-2A68-4ADA-820C-D4F2E25DC768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD4A52F-5090-4168-8F38-72B169BFFA77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Demand Table" sheetId="4" r:id="rId1"/>
@@ -730,11 +730,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -953,7 +953,7 @@
   <dimension ref="A1:S1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -969,7 +969,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="49"/>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="70" t="s">
         <v>69</v>
       </c>
       <c r="C1" s="49"/>
@@ -1035,7 +1035,7 @@
       <c r="L2" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="70"/>
+      <c r="M2" s="72"/>
     </row>
     <row r="3" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
@@ -1134,7 +1134,7 @@
     </row>
     <row r="8" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="49"/>
-      <c r="B8" s="72"/>
+      <c r="B8" s="70"/>
       <c r="C8" s="49"/>
       <c r="D8" s="25" t="s">
         <v>19</v>
@@ -1154,7 +1154,7 @@
     </row>
     <row r="9" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="49"/>
-      <c r="B9" s="72" t="s">
+      <c r="B9" s="70" t="s">
         <v>70</v>
       </c>
       <c r="C9" s="49"/>
@@ -1360,7 +1360,7 @@
       <c r="B19" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="70"/>
+      <c r="C19" s="72"/>
       <c r="D19" s="17">
         <f>SUM(D10:D18)</f>
         <v>16449</v>

</xml_diff>